<commit_message>
Add database dump and finalize query scripts
</commit_message>
<xml_diff>
--- a/res/Results.xlsx
+++ b/res/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>1950-1959</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Jazz</t>
+  </si>
+  <si>
+    <t>[0-90]</t>
+  </si>
+  <si>
+    <t>[91-180]</t>
+  </si>
+  <si>
+    <t>[181-240]</t>
+  </si>
+  <si>
+    <t>[241-300]</t>
+  </si>
+  <si>
+    <t>[301-360]</t>
+  </si>
+  <si>
+    <t>[361-…]</t>
   </si>
 </sst>
 </file>
@@ -208,6 +226,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -223,6 +246,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -238,6 +266,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -253,6 +286,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -268,6 +306,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -283,6 +326,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -300,6 +348,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-327B-4CDD-95F4-D5166A206E4B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -885,6 +938,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -900,6 +958,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -915,6 +978,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -930,6 +998,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -945,6 +1018,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -960,6 +1038,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1011,6 +1094,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1026,6 +1114,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1041,6 +1134,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1056,6 +1154,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1071,6 +1174,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1086,6 +1194,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6129-404A-925C-DCB6A16A7196}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1170,6 +1283,331 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Zadatak</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> 3. c) Broj pesama prema trajanju[s].</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$34:$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>[0-90]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[91-180]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[181-240]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[241-300]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[301-360]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>[361-…]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$34:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2524</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BA5-4FBE-8BB4-630CD7B7E462}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="964902767"/>
+        <c:axId val="963316607"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="964902767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="963316607"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="963316607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="964902767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1334,6 +1772,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -2535,6 +3013,511 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2982,6 +3965,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{988E1A0A-F65E-4764-B072-B410834F8268}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3253,10 +4272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3416,6 +4435,54 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>